<commit_message>
görsel alımı da çok iyi
</commit_message>
<xml_diff>
--- a/technomarket/TechnoMarket_Urunler.xlsx
+++ b/technomarket/TechnoMarket_Urunler.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1192,10 +1192,8 @@
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>09225074</t>
-        </is>
+      <c r="B12" t="n">
+        <v>9225074</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1263,10 +1261,8 @@
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>09218978</t>
-        </is>
+      <c r="B13" t="n">
+        <v>9218978</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1334,10 +1330,8 @@
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>09216193</t>
-        </is>
+      <c r="B14" t="n">
+        <v>9216193</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1405,10 +1399,8 @@
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>09188047</t>
-        </is>
+      <c r="B15" t="n">
+        <v>9188047</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1472,10 +1464,8 @@
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>09175143</t>
-        </is>
+      <c r="B16" t="n">
+        <v>9175143</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1536,6 +1526,297 @@
         </is>
       </c>
       <c r="O16" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-x1126ah-09175143</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>09225074</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>XMART TAŞINABİLİR MULTİMEDYA PROJEKTÖR MPP-40</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>169</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>XMART</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8bd2191.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8d5e802.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8f76bb7.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f9188007.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/xmart-portable-multimedia-projector-mpp-40-09225074</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>09218978</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>EPSON CO-W01</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>699</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>EPSON</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8c99b73e.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8cbaed42.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d0c2b08.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d32d971.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d59627a.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d8b2bb5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/epson-co-w01-09218978</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09216193</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SAMSUNG SP-LFF3CLA SERBEST STİL AKILLI</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1099</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb152806d.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb16b6442.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1869b71.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1a0cf19.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1d67ef1.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb20b69a1.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/samsung-sp-lff3cla-the-freestyle-smart-09216193</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09188047</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR X128HP</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>819</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09188047/6077de34291d4.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-x128hp-09188047</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09175143</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR X1126AH</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>728</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09175143/5d415857e49d5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09175143/5d4158592eb69.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
         <is>
           <t>https://www.technomarket.bg/proektori/acer-projector-x1126ah-09175143</t>
         </is>

</xml_diff>

<commit_message>
gayet güzel ama timeout yok
</commit_message>
<xml_diff>
--- a/technomarket/TechnoMarket_Urunler.xlsx
+++ b/technomarket/TechnoMarket_Urunler.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,15 +516,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>09225074</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3800202099607</t>
-        </is>
+      <c r="A2" t="n">
+        <v>9225074</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3800202099607</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -593,15 +589,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>09218978</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>8715946706849</t>
-        </is>
+      <c r="A3" t="n">
+        <v>9218978</v>
+      </c>
+      <c r="B3" t="n">
+        <v>8715946706849</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -680,15 +672,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>09216193</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>8806094951776</t>
-        </is>
+      <c r="A4" t="n">
+        <v>9216193</v>
+      </c>
+      <c r="B4" t="n">
+        <v>8806094951776</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -756,15 +744,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>09188047</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5557678898987</t>
-        </is>
+      <c r="A5" t="n">
+        <v>9188047</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5557678898987</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -812,15 +796,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>09175143</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4710180062793</t>
-        </is>
+      <c r="A6" t="n">
+        <v>9175143</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4710180062793</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -875,6 +855,2672 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>9225101</v>
+      </c>
+      <c r="B7" t="n">
+        <v>8806095545325</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SAMSUNG SP-LPU9D PREMIERE AKILLI 4K</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>9399</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0bf83676.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c150678.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c37cbd0.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c6031a3.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c7db33a.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0ca893e0.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/samsung-sp-lpu9d-premiere-smart-4k-09225101</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>EKRAN BOYUTU: 100 ila 130" (254-330 CM)
+ÇÖZÜNÜRLÜK: 4K ULTRA HD 3840 x 2160
+Üçlü lazer teknolojisi
+Kuantum İşlemci 4K
+Parlaklık (ISO Lümen): 3450 lümen
+Kuantum HDR, HDR 10+, HLG
+Gerçek Derinlik Artırıcı
+Game Motion Plus, Süper Ultra Geniş Oyun Görünümü
+İŞLETİM SİSTEMİ: Tizen™
+Bluetooth, Wi-Fi Doğrudan
+HDMIX3, USBX1
+RADYO: DVB-T2/C/S2
+Uyarlanabilir Ses Pro, Q-Senfoni
+Dolby Atmos, 360 Ses
+SES 40 W -2.2.2CH</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>9173388</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4713883197915</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR P5630</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1649</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09173388/5ceb98fe9c1c8.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-p5630-09173388</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+KONTRAST: 20.000:1
+ÇÖZÜNÜRLÜK: 1920x1200
+TEKNOLOJİ: DLP
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9218979</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8715946706825</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>EPSON CO-FH01</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>999</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>EPSON</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e910db0f7.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91698a75.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e919b4ad5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91c2d611.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91eb83cd.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e92147c80.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/epson-co-fh01-09218979</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+ÇÖZÜNÜRLÜK: 1920 X 1080 (FullHD)
+FORMAT: 16:9
+EKRAN BOYUTU: 26 - 391"
+TASARIM MESAFESİ: 1,64 m.
+PARLAKLIK: 3000 lm
+RENK ARALIĞI: 16,77 m.
+TEKNOLOJİ: LCD
+LAMBA ÖMRÜ: 6000 saat.
+YÜKSEK HOPARLÖRLER: VAR
+BAĞLANTI NOKTALARI: HDMI 1.4, USB 2.0
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9228841</v>
+      </c>
+      <c r="B10" t="n">
+        <v>6942351409382</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>HISENSE Hisense C2 4K 2000lm</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2649</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Projektörler</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>HISENSE</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b5b77def.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b560b36b.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b62b6adc.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b6503121.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b67bf495.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b6a11cc3.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/hisense-c2-4k-2000-lm-09228841</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Maksimum çözünürlük: Ultra HD 3840x2160
+Frekans: 50 Hz, 60 Hz
+Kontrast: 1700:1
+HLD teknolojisi: Evet
+Dolby Vision: Evet
+Ultra HD'ye Yayınlama: Evet
+Oyunlar modunda gecikme: 60 ms
+Çıkış gücü: 2x10 W
+Ses teknolojisi: DTS Virtual X, DTS HD
+Temel uygulamalar: Netflix, YouTube, Prime Video, Disney+, FIFA+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9218598</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3800916014309</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NEO LED-32H3M HD LED TV</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>199</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>32"_42"</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/65646423cde97.png.webp</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564642793d6b.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564642f4576a.png.webp</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/65646431d5ffc.png.webp</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564643637738.png.webp</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564643857bca.png.webp</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-32h3m-hd-led-tv-09218598</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>NEO LED-32H3M HD LED TV
+32" (81 CM) EKRAN BOYUTU
+1366X768 DPI HD ÇÖZÜNÜRLÜK
+PARLAKLIK 200 PPI
+KONTRAST 4000:1
+AÇI - 178°X178°
+3XHDMI, 2XUSB, CI</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9218599</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3800916014262</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NEO LED-32HS3M HD AKILLI TV</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>249</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>32"_42"</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218599/6564666f097f3.png.webp</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218599/6564666ae17b9.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218599/656466725da0c.png.webp</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218599/656466753ef63.png.webp</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218599/656466780194e.png.webp</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218599/6564667a2469b.png.webp</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-32hs3m-hd-smart-tv-09218599</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>NEO LED-32HS3M HD AKILLI TV
+32" (81 CM) EKRAN BOYUTU
+ÇÖZÜNÜRLÜK 1366X768 DPI HD
+AKILLI TV, AÇIK İŞLETİM SİSTEMİ
+PARLAKLIK 200 PPI, KONTRAST 4000:1
+AÇI - 178°X178°
+3XHDMI, 2XUSB, CI</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>9205136</v>
+      </c>
+      <c r="B13" t="n">
+        <v>8806091636959</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>LG 32LQ63006LA FHD LED AKILLI TV</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>349</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>32"_42"</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>LG</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09205136/62eb892dd5910.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09205136/621752923bd44.png.webp</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09205136/6217526c0c55e.png.webp</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09205136/621752703edc7.png.webp</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09205136/62175272cefd3.png.webp</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09205136/621752765a892.png.webp</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/lg-32lq63006la-fhd-led-smart-tv-09205136</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>LG 32LQ63006LA FHD LED AKILLI TV
+32"(81 CM) EKRAN BOYUTU
+1920X1080 FULL HD ÇÖZÜNÜRLÜK
+α5 GEN 5 AI İŞLEMCİ
+İŞLETİM SİSTEMİ: WEBOS
+TEKNOLOJİLER AKTİF HDR, HLG
+TEKNOLOJİ HDR10 Pro
+FILMMAKER MODE™ TEKNOLOJİSİ
+THİNQ ÖZELLİĞİ
+ENERJİ SINIFI: F</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>9212936</v>
+      </c>
+      <c r="B14" t="n">
+        <v>8806094908558</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SAMSUNG UE-32T4302AE HD AKILLI TV</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>349</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>32"_42"</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09212936/641b071db5026.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09212936/641b071f384a9.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09212936/641b07343c39e.png.webp</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09212936/641b0735f246c.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/samsung-ue-32t4302ae-hd-smart-tv-09212936</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>32" (81 CM) HD AKILLI TV
+EKRAN BOYUTU 32" (81CM)
+ÇÖZÜNÜRLÜK: 1366X768
+EKRAN TEKNOLOJİSİ: LED
+PurColor, Ultra Temiz Görünüm
+AKILLI TV, DAHİLİ WI-FI
+DİJİTAL TUNER: DVB-T2/C
+HDMI X 2, USB X 1, KOMPOZİT GİRİŞ (AV), KOMPONENT GİRİŞ
+Enerji sınıfı: F</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>9229138</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8806097118527</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SAMSUNG QE-43Q7F QLED AKILLI TV</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>699</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>43"_49"</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229138/6810c985227d9.png.webp</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229138/6810c9a59a70b.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229138/6810c986c6f10.png.webp</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229138/6810c988d54a0.png.webp</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229138/6810c98c4ee16.png.webp</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229138/6810c98f40247.png.webp</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/samsung-qe-43q7f-qled-smart-tv-09229138</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>EKRAN TEKNOLOJİSİ: QLED
+EKRAN BOYUTU 43" (109 CM)
+ÇÖZÜNÜRLÜK: 4K ULTRA HD 3840 X 2160
+Q4 Yapay Zeka İşlemcisi
+Kuantum HDR, Mega Kontrast
+Üstün UHD Karartma, 4K Yükseltme
+Renk Güçlendirici Pro
+DİJİTAL TUNER DVB-T2/C/S2
+BLUETOOTH, WI-FI
+Tizen™ Akıllı TV
+HDMI, USB, CI+(1.4)
+SES: 20W, 2CH
+OTS Lite, Q-Senfoni
+Enerji sınıfı: G</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>9227153</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3800916015399</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NEO LED-24S25M HD AKILLI LED TV</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>209</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>32"'e kadar</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227153/67b47803e8dd4.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227153/67b47806ad174.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227153/67b4780a5d875.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227153/67b4780cbdf9e.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227153/67b4780f67b2c.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227153/67b4781183519.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-24s25m-hd-smart-led-tv-09227153</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>NEO LED-24S25M HD AKILLI LED TV
+24" (60 CM) EKRAN BOYUTU
+1366X768 HD ÇÖZÜNÜRLÜK
+PARLAKLIK -150 (cd/m)
+KONTRAST - 3000:1
+AKILLI TV, AÇIK İŞLETİM SİSTEMİ
+HDMI, USB, CI"</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>9227156</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3800916015429</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NEO LED-55US25M UHD AKILLI LED TV</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>649</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>50"_55"</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227156/67b4797ab68f2.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227156/67b4797d268c9.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227156/67b4797fdfbe5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227156/67b47985b0eb7.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227156/67b47988cf827.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227156/67b4798b75a67.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-55us25m-uhd-smart-led-tv-09227156</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>NEO LED-55US25M UHD AKILLI LED TV
+55" (139 CM) EKRAN BOYUTU
+3840X2160 FHD ÇÖZÜNÜRLÜK
+PARLAKLIK -220 (cd/m)
+KONTRAST - 3000:1
+AKILLI TV, AÇIK İŞLETİM SİSTEMİ
+HDMI, USB, CI</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>9218600</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3800916014279</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NEO LED-43FS3M FHD AKILLI TV</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>399</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>43"_49"</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218600/656485124cbae.png.webp</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218600/656485168def8.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218600/65648527b76a3.png.webp</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218600/6564852abfde9.png.webp</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218600/6564852ee6070.png.webp</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218600/656485320ea43.png.webp</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-43fs3m-fhd-smart-tv-09218600</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>NEO LED-43FS3M FHD AKILLI TV
+43" (109 CM) EKRAN BOYUTU
+1920X1080 FHD ÇÖZÜNÜRLÜK
+AÇIK İŞLETİM SİSTEMİ
+PARLAKLIK 220 PPI
+KONTRAST 3000:1
+AÇI - 178°X178°
+3XHDMI, 2XUSB, CI, RJ45</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>9229322</v>
+      </c>
+      <c r="B19" t="n">
+        <v>5901292526023</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>TCL 40S5K FHD QLED AKILLI TV ANDROID</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>419</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>32"_42"</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>TCL</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229322/682d91a81a5b5.png.webp</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229322/682d91e734d88.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229322/682d91a9da72f.png.webp</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229322/682d91abaa206.png.webp</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229322/682d91b19d5d3.png.webp</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229322/682d91b7383a3.png.webp</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/tcl-40s5k-fhd-qled-smart-tv-android-09229322</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>FHD QLED AKILLI TV
+EKRAN BOYUTU 40" (101 CM)
+ÇÖZÜNÜRLÜK: FHD 1920X1080
+İşlemci Dört Çekirdekli
+Kuantum Noktası
+ÜFE 1000
+DİJİTAL TUNER DVB-T2/C/S2
+AKILLI TV
+AndroidTV
+SES: 2 x 10W
+Bluetooth, HDMI X 2, USB X 1
+Enerji sınıfı: F</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>9229323</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5901292526030</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>TCL 32S5K FHD QLED AKILLI TV ANDROID</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>349</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>32"_42"</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>TCL</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229323/682d9134d5510.png.webp</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229323/682d916bc0e12.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229323/682d913b68bdc.png.webp</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229323/682d913e85987.png.webp</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229323/682d91420bf0c.png.webp</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09229323/682d914c0d790.png.webp</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/tcl-32s5k-fhd-qled-smart-tv-android-09229323</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>FHD QLED AKILLI TV
+EKRAN BOYUTU 32" (81 CM)
+ÇÖZÜNÜRLÜK: FHD 1920X1080
+İşlemci Dört Çekirdekli
+Kuantum Noktası
+ÜFE 1000
+DİJİTAL TUNER DVB-T2/C/S2
+AKILLI TV
+AndroidTV
+SES: 2 x 8W
+Bluetooth, HDMI X 2, USB X 1
+Enerji sınıfı: F</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>9227151</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3800916015375</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NEO LED-24B25M HD LED TV</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>189</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>32"'e kadar</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227151/67b477266e627.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227151/67b47729db9ed.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227151/67b4772cb1972.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227151/67b4772f355a3.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227151/67b477317e9ea.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09227151/67b477341303f.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-24b25m-hd-led-tv-09227151</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>NEO LED-24B12VM HD LED TV
+24" (61 CM) EKRAN BOYUTU
+1366X768 HD ÇÖZÜNÜRLÜK
+PARLAKLIK - 200 PPI,
+KONTRAST - 3000:1
+HDMI, USB, CI</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>9225074</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3800202099607</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>XMART TAŞINABİLİR MULTİMEDYA PROJEKTÖR MPP-40</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>169</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>XMART</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8bd2191.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8d5e802.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8f76bb7.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f9188007.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/xmart-portable-multimedia-projector-mpp-40-09225074</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>30W LED lambalı (280 ANSI Lümen) multimedya projektörü.
+LED lamba ömrü: 50.000 saat.
+Akıllı telefon/tablet ekranının projektöre kablosuz aktarımı (Yansıtma).
+Önceden yüklenmiş multimedya oynatıcıya ve Google Play'den uygulama ekleme özelliğine sahip Android 11 işletim sistemi.
+Projeksiyon boyutu: 130″'ye (330 cm) kadar.
+Otomatik trapezoid düzeltme ve hassas manuel odak ayarı.
+Çözünürlük: 1280 x 720 piksel, 4K@30fps'yi destekler.
+USB Flash bellekten veya HDMI girişi aracılığıyla oynatma.
+Kulaklık bağlamak için dahili 3W hoparlör ve 3,5 mm ses çıkışı.
+Uzaktan kumandayla tamamlayın.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>9218978</v>
+      </c>
+      <c r="B23" t="n">
+        <v>8715946706849</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>EPSON CO-W01</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>699</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>EPSON</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8c99b73e.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8cbaed42.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d0c2b08.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d32d971.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d59627a.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d8b2bb5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/epson-co-w01-09218978</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+ÇÖZÜNÜRLÜK: 1200 X 800(WXGA)
+FORMAT: 16:10
+EKRAN BOYUTU: 25 - 378"
+TASARIM MESAFESİ: 1,64 m.
+PARLAKLIK: 3000 lm
+RENK ARALIĞI: 16,77 m.
+TEKNOLOJİ: LCD
+LAMBA ÖMRÜ: 6000 saat.
+YÜKSEK HOPARLÖRLER: VAR
+BAĞLANTI NOKTALARI: HDMI 1.4, USB 2.0
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>9216193</v>
+      </c>
+      <c r="B24" t="n">
+        <v>8806094951776</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>SAMSUNG SP-LFF3CLA SERBEST STİL AKILLI</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1099</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb152806d.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb16b6442.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1869b71.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1a0cf19.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1d67ef1.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb20b69a1.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/samsung-sp-lff3cla-the-freestyle-smart-09216193</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>EKRAN BOYUTU: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>9188047</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5557678898987</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR X128HP</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>819</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09188047/6077de34291d4.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-x128hp-09188047</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>9175143</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4710180062793</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR X1126AH</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>728</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09175143/5d415857e49d5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09175143/5d4158592eb69.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-x1126ah-09175143</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+KONTRAST: 20.000:1
+ÇÖZÜNÜRLÜK: 800x600
+TEKNOLOJİ: DLP
+RENK: SİYAH</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>9225101</v>
+      </c>
+      <c r="B27" t="n">
+        <v>8806095545325</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SAMSUNG SP-LPU9D PREMIERE AKILLI 4K</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>9399</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0bf83676.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c150678.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c37cbd0.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c6031a3.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c7db33a.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0ca893e0.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/samsung-sp-lpu9d-premiere-smart-4k-09225101</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>EKRAN BOYUTU: 100 ila 130" (254-330 CM)
+ÇÖZÜNÜRLÜK: 4K ULTRA HD 3840 x 2160
+Üçlü lazer teknolojisi
+Kuantum İşlemci 4K
+Parlaklık (ISO Lümen): 3450 lümen
+Kuantum HDR, HDR 10+, HLG
+Gerçek Derinlik Artırıcı
+Game Motion Plus, Süper Ultra Geniş Oyun Görünümü
+İŞLETİM SİSTEMİ: Tizen™
+Bluetooth, Wi-Fi Doğrudan
+HDMIX3, USBX1
+RADYO: DVB-T2/C/S2
+Uyarlanabilir Ses Pro, Q-Senfoni
+Dolby Atmos, 360 Ses
+SES 40 W -2.2.2CH</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>9173388</v>
+      </c>
+      <c r="B28" t="n">
+        <v>4713883197915</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR P5630</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1649</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09173388/5ceb98fe9c1c8.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-p5630-09173388</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+KONTRAST: 20.000:1
+ÇÖZÜNÜRLÜK: 1920x1200
+TEKNOLOJİ: DLP
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>9218979</v>
+      </c>
+      <c r="B29" t="n">
+        <v>8715946706825</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>EPSON CO-FH01</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>999</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>EPSON</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e910db0f7.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91698a75.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e919b4ad5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91c2d611.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91eb83cd.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e92147c80.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/epson-co-fh01-09218979</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+ÇÖZÜNÜRLÜK: 1920 X 1080 (FullHD)
+FORMAT: 16:9
+EKRAN BOYUTU: 26 - 391"
+TASARIM MESAFESİ: 1,64 m.
+PARLAKLIK: 3000 lm
+RENK ARALIĞI: 16,77 m.
+TEKNOLOJİ: LCD
+LAMBA ÖMRÜ: 6000 saat.
+YÜKSEK HOPARLÖRLER: VAR
+BAĞLANTI NOKTALARI: HDMI 1.4, USB 2.0
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>9228841</v>
+      </c>
+      <c r="B30" t="n">
+        <v>6942351409382</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>HISENSE Hisense C2 4K 2000lm</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2649</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>HISENSE</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b5b77def.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b560b36b.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b62b6adc.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b6503121.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b67bf495.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b6a11cc3.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/hisense-c2-4k-2000-lm-09228841</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Maksimum çözünürlük: Ultra HD 3840x2160
+Frekans: 50 Hz, 60 Hz
+Kontrast: 1700:1
+HLD teknolojisi: Evet
+Dolby Vision: Evet
+Ultra HD'ye Yayınlama: Evet
+Oyunlar modunda gecikme: 60 ms
+Çıkış gücü: 2x10 W
+Ses teknolojisi: DTS Virtual X, DTS HD
+Temel uygulamalar: Netflix, YouTube, Prime Video, Disney+, FIFA+</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>9218598</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3800916014309</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>NEO LED-32H3M HD LED TV</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>199</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Televizyonlar &gt; 32 "_ 42 "</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/65646423cde97.png.webp</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564642793d6b.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564642f4576a.png.webp</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/65646431d5ffc.png.webp</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564643637738.png.webp</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564643857bca.png.webp</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-32h3m-hd-led-tv-09218598</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>NEO LED-32H3M HD LED TV
+32" (81 CM) EKRAN BOYUTU
+1366X768 DPI HD ÇÖZÜNÜRLÜK
+PARLAKLIK 200 PPI
+KONTRAST 4000:1
+AÇI - 178°X178°
+3XHDMI, 2XUSB, CI</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>09225074</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>3800202099607</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>XMART TAŞINABİLİR MULTİMEDYA PROJEKTÖR MPP-40</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>169</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>XMART</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8bd2191.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8d5e802.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f8f76bb7.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225074/67188f9188007.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/xmart-portable-multimedia-projector-mpp-40-09225074</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>30W LED lambalı (280 ANSI Lümen) multimedya projektörü.
+LED lamba ömrü: 50.000 saat.
+Akıllı telefon/tablet ekranının projektöre kablosuz aktarımı (Yansıtma).
+Önceden yüklenmiş multimedya oynatıcıya ve Google Play'den uygulama ekleme özelliğine sahip Android 11 işletim sistemi.
+Projeksiyon boyutu: 130″'ye (330 cm) kadar.
+Otomatik trapezoid düzeltme ve hassas manuel odak ayarı.
+Çözünürlük: 1280 x 720 piksel, 4K@30fps'yi destekler.
+USB Flash bellekten veya HDMI girişi aracılığıyla oynatma.
+Kulaklık bağlamak için dahili 3W hoparlör ve 3,5 mm ses çıkışı.
+Uzaktan kumandayla tamamlayın.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>09218978</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>8715946706849</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>EPSON CO-W01</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>699</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>EPSON</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8c99b73e.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8cbaed42.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d0c2b08.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d32d971.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d59627a.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218978/6618e8d8b2bb5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/epson-co-w01-09218978</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+ÇÖZÜNÜRLÜK: 1200 X 800(WXGA)
+FORMAT: 16:10
+EKRAN BOYUTU: 25 - 378"
+TASARIM MESAFESİ: 1,64 m.
+PARLAKLIK: 3000 lm
+RENK ARALIĞI: 16,77 m.
+TEKNOLOJİ: LCD
+LAMBA ÖMRÜ: 6000 saat.
+YÜKSEK HOPARLÖRLER: VAR
+BAĞLANTI NOKTALARI: HDMI 1.4, USB 2.0
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>09216193</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>8806094951776</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>SAMSUNG SP-LFF3CLA SERBEST STİL AKILLI</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1099</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb152806d.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb16b6442.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1869b71.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1a0cf19.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb1d67ef1.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09216193/64eceb20b69a1.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/samsung-sp-lff3cla-the-freestyle-smart-09216193</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>EKRAN BOYUTU: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>09188047</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>5557678898987</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR X128HP</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>819</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09188047/6077de34291d4.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-x128hp-09188047</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>09175143</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>4710180062793</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR X1126AH</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>728</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09175143/5d415857e49d5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09175143/5d4158592eb69.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-x1126ah-09175143</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+KONTRAST: 20.000:1
+ÇÖZÜNÜRLÜK: 800x600
+TEKNOLOJİ: DLP
+RENK: SİYAH</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>09225101</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>8806095545325</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>SAMSUNG SP-LPU9D PREMIERE AKILLI 4K</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>9399</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0bf83676.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c150678.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c37cbd0.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c6031a3.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0c7db33a.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09225101/670fa0ca893e0.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/samsung-sp-lpu9d-premiere-smart-4k-09225101</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>EKRAN BOYUTU: 100 ila 130" (254-330 CM)
+ÇÖZÜNÜRLÜK: 4K ULTRA HD 3840 x 2160
+Üçlü lazer teknolojisi
+Kuantum İşlemci 4K
+Parlaklık (ISO Lümen): 3450 lümen
+Kuantum HDR, HDR 10+, HLG
+Gerçek Derinlik Artırıcı
+Game Motion Plus, Süper Ultra Geniş Oyun Görünümü
+İŞLETİM SİSTEMİ: Tizen™
+Bluetooth, Wi-Fi Doğrudan
+HDMIX3, USBX1
+RADYO: DVB-T2/C/S2
+Uyarlanabilir Ses Pro, Q-Senfoni
+Dolby Atmos, 360 Ses
+SES 40 W -2.2.2CH</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>09173388</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>4713883197915</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ACER PROJEKTÖR P5630</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1649</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09173388/5ceb98fe9c1c8.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/acer-projector-p5630-09173388</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+KONTRAST: 20.000:1
+ÇÖZÜNÜRLÜK: 1920x1200
+TEKNOLOJİ: DLP
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>09218979</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>8715946706825</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>EPSON CO-FH01</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>999</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>EPSON</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e910db0f7.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91698a75.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e919b4ad5.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91c2d611.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e91eb83cd.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218979/6618e92147c80.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/epson-co-fh01-09218979</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>PROJEKTÖR
+ÇÖZÜNÜRLÜK: 1920 X 1080 (FullHD)
+FORMAT: 16:9
+EKRAN BOYUTU: 26 - 391"
+TASARIM MESAFESİ: 1,64 m.
+PARLAKLIK: 3000 lm
+RENK ARALIĞI: 16,77 m.
+TEKNOLOJİ: LCD
+LAMBA ÖMRÜ: 6000 saat.
+YÜKSEK HOPARLÖRLER: VAR
+BAĞLANTI NOKTALARI: HDMI 1.4, USB 2.0
+RENK: BEYAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>09228841</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>6942351409382</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>HISENSE Hisense C2 4K 2000lm</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2649</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Projektörler</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>HISENSE</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b5b77def.jpg.webp</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b560b36b.jpg.webp</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b62b6adc.jpg.webp</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b6503121.jpg.webp</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b67bf495.jpg.webp</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09228841/67ff4b6a11cc3.jpg.webp</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/proektori/hisense-c2-4k-2000-lm-09228841</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Maksimum çözünürlük: Ultra HD 3840x2160
+Frekans: 50 Hz, 60 Hz
+Kontrast: 1700:1
+HLD teknolojisi: Evet
+Dolby Vision: Evet
+Ultra HD'ye Yayınlama: Evet
+Oyunlar modunda gecikme: 60 ms
+Çıkış gücü: 2x10 W
+Ses teknolojisi: DTS Virtual X, DTS HD
+Temel uygulamalar: Netflix, YouTube, Prime Video, Disney+, FIFA+</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>09218598</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>3800916014309</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>NEO LED-32H3M HD LED TV</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>199</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>BGN</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>TV, Ses ve Elektronik &gt; Televizyonlar &gt; 32 "_ 42 "</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>NEO</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/65646423cde97.png.webp</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564642793d6b.JPG.webp</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564642f4576a.png.webp</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/65646431d5ffc.png.webp</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564643637738.png.webp</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>https://cdn.technomarket.bg/ng/media/cache/mid_thumb/uploads/library/product/09218598/6564643857bca.png.webp</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>https://www.technomarket.bg/televizor/neo-led-32h3m-hd-led-tv-09218598</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>NEO LED-32H3M HD LED TV
+32" (81 CM) EKRAN BOYUTU
+1366X768 DPI HD ÇÖZÜNÜRLÜK
+PARLAKLIK 200 PPI
+KONTRAST 4000:1
+AÇI - 178°X178°
+3XHDMI, 2XUSB, CI</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>